<commit_message>
new rules of blocking added per piece
</commit_message>
<xml_diff>
--- a/Rules, Resources and extras.xlsx
+++ b/Rules, Resources and extras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HermiloOrtega\Dropbox\CICCC\WMAD\202 Java\ChessGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB5133C9-B1AE-437A-891B-3E06BE8EE97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471C2A54-85BC-41C2-ABE8-1BD69FB97C8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{2E2135E0-951D-4716-9FC6-9493C47D7665}"/>
+    <workbookView xWindow="-20610" yWindow="8460" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{2E2135E0-951D-4716-9FC6-9493C47D7665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="190">
   <si>
     <t>A</t>
   </si>
@@ -3227,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC3A6DC-A236-4D9D-8E44-3B79F1FEE04F}">
-  <dimension ref="B3:AG31"/>
+  <dimension ref="A3:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3238,7 +3238,7 @@
     <col min="1" max="16384" width="4.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>8</v>
       </c>
@@ -3249,18 +3249,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K4" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V4" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG4" s="28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3306,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>175</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B7" s="39" t="s">
         <v>173</v>
       </c>
@@ -3391,16 +3391,16 @@
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="39" t="s">
         <v>173</v>
       </c>
       <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="6"/>
+      <c r="AD7" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE7" s="1"/>
       <c r="AF7" s="8">
         <v>6</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="13" t="s">
         <v>174</v>
@@ -3448,17 +3448,17 @@
         <v>3</v>
       </c>
       <c r="X8" s="4"/>
-      <c r="Y8" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
+      <c r="AA8" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="6"/>
+      <c r="AE8" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="AF8" s="8">
         <v>5</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="13" t="s">
         <v>174</v>
@@ -3520,15 +3520,15 @@
         <v>4</v>
       </c>
       <c r="X9" s="17"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18" t="s">
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
       <c r="AD9" s="18"/>
-      <c r="AE9" s="19"/>
+      <c r="AE9" s="18"/>
       <c r="AF9" s="8">
         <v>4</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
         <v>173</v>
       </c>
@@ -3570,17 +3570,17 @@
         <v>5</v>
       </c>
       <c r="X10" s="17"/>
-      <c r="Y10" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="AB10" s="18"/>
-      <c r="AC10" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="AC10" s="18"/>
       <c r="AD10" s="18"/>
-      <c r="AE10" s="19"/>
+      <c r="AE10" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="AF10" s="8">
         <v>3</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>175</v>
       </c>
@@ -3625,16 +3625,16 @@
       </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="18"/>
-      <c r="Z11" s="39" t="s">
-        <v>173</v>
-      </c>
+      <c r="Z11" s="1"/>
       <c r="AA11" s="18"/>
       <c r="AB11" s="39" t="s">
         <v>173</v>
       </c>
       <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="19"/>
+      <c r="AD11" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE11" s="18"/>
       <c r="AF11" s="8">
         <v>2</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3688,7 +3688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>0</v>
       </c>
@@ -3768,7 +3768,10 @@
       <c r="AF13" s="32"/>
       <c r="AG13" s="32"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="B14" s="32">
         <v>0</v>
       </c>
@@ -3795,6 +3798,9 @@
       </c>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
+      <c r="L14" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="M14" s="32">
         <v>0</v>
       </c>
@@ -3821,6 +3827,9 @@
       </c>
       <c r="U14" s="32"/>
       <c r="V14" s="32"/>
+      <c r="W14" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="X14" s="32">
         <v>0</v>
       </c>
@@ -3848,7 +3857,7 @@
       <c r="AF14" s="32"/>
       <c r="AG14" s="32"/>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
         <v>185</v>
       </c>
@@ -3877,7 +3886,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D16" s="27" t="s">
         <v>183</v>
       </c>
@@ -3903,7 +3912,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
         <v>10</v>
       </c>
@@ -3914,18 +3923,18 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K19" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V19" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG19" s="28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -3975,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B21" s="39" t="s">
         <v>173</v>
       </c>
@@ -4029,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="39" t="s">
         <v>173</v>
@@ -4083,7 +4092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="1"/>
       <c r="D23" s="39" t="s">
@@ -4143,7 +4152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -4211,7 +4220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
       <c r="D25" s="39" t="s">
@@ -4271,7 +4280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="39" t="s">
         <v>173</v>
@@ -4325,7 +4334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="39" t="s">
         <v>173</v>
       </c>
@@ -4379,7 +4388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>0</v>
       </c>
@@ -4459,7 +4468,10 @@
       <c r="AF28" s="32"/>
       <c r="AG28" s="32"/>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="B29" s="32">
         <v>0</v>
       </c>
@@ -4486,6 +4498,9 @@
       </c>
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
+      <c r="L29" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="M29" s="32">
         <v>0</v>
       </c>
@@ -4512,6 +4527,9 @@
       </c>
       <c r="U29" s="32"/>
       <c r="V29" s="32"/>
+      <c r="W29" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="X29" s="32">
         <v>0</v>
       </c>
@@ -4539,7 +4557,7 @@
       <c r="AF29" s="32"/>
       <c r="AG29" s="32"/>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B30" s="27" t="s">
         <v>188</v>
       </c>
@@ -4550,7 +4568,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
         <v>187</v>
       </c>

</xml_diff>